<commit_message>
Invalid Login -Data From XL
</commit_message>
<xml_diff>
--- a/src/test/resources/data/input.xlsx
+++ b/src/test/resources/data/input.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\B24\Day32 Dec22\B24\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67CB9E03-5BD8-4686-BE29-B890618F304B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{130F112C-8CB3-46AE-9538-E2418C941E88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5070" yWindow="615" windowWidth="15255" windowHeight="9030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3165" yWindow="3330" windowWidth="15255" windowHeight="6660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ValidLogin" sheetId="1" r:id="rId1"/>
+    <sheet name="InvalidLogin" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,9 +26,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>admin</t>
+  </si>
+  <si>
+    <t>manager</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>FailMsg</t>
+  </si>
+  <si>
+    <t>Home Page is not displayed</t>
+  </si>
+  <si>
+    <t>abcd</t>
+  </si>
+  <si>
+    <t>xyz</t>
+  </si>
+  <si>
+    <t>Err MSg is not displayed</t>
   </si>
 </sst>
 </file>
@@ -345,17 +370,78 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F531828D-8EFE-416A-9671-F0FB5D10125F}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="22.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>